<commit_message>
Edit the 511.org GTFS
</commit_message>
<xml_diff>
--- a/input-data/NYE timetables.xlsx
+++ b/input-data/NYE timetables.xlsx
@@ -11,105 +11,171 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
   <si>
     <t>Route</t>
   </si>
   <si>
+    <t>Local Weekday</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>SF</t>
+  </si>
+  <si>
+    <t>22 St</t>
+  </si>
+  <si>
+    <t>Bayshore</t>
+  </si>
+  <si>
+    <t>S SF</t>
+  </si>
+  <si>
+    <t>San Bruno</t>
+  </si>
+  <si>
+    <t>Millbrae</t>
+  </si>
+  <si>
+    <t>Burlingame</t>
+  </si>
+  <si>
+    <t>San Mateo</t>
+  </si>
+  <si>
+    <t>Hayward Park</t>
+  </si>
+  <si>
+    <t>Hillsdale</t>
+  </si>
+  <si>
+    <t>Belmont</t>
+  </si>
+  <si>
+    <t>San Carlos</t>
+  </si>
+  <si>
+    <t>Redwood City</t>
+  </si>
+  <si>
+    <t>Menlo Park</t>
+  </si>
+  <si>
+    <t>Palo Alto</t>
+  </si>
+  <si>
+    <t>California Ave</t>
+  </si>
+  <si>
+    <t>San Antonio</t>
+  </si>
+  <si>
+    <t>Mountain View</t>
+  </si>
+  <si>
+    <t>Sunnyvale</t>
+  </si>
+  <si>
+    <t>Lawrence</t>
+  </si>
+  <si>
+    <t>Santa Clara</t>
+  </si>
+  <si>
+    <t>San Jose Diridon</t>
+  </si>
+  <si>
+    <t>Stop ID</t>
+  </si>
+  <si>
+    <t>san_francisco</t>
+  </si>
+  <si>
+    <t>22nd_street</t>
+  </si>
+  <si>
+    <t>bayshore</t>
+  </si>
+  <si>
+    <t>south_sf</t>
+  </si>
+  <si>
+    <t>san_bruno</t>
+  </si>
+  <si>
+    <t>millbrae</t>
+  </si>
+  <si>
+    <t>burlingame</t>
+  </si>
+  <si>
+    <t>san_mateo</t>
+  </si>
+  <si>
+    <t>hayward_park</t>
+  </si>
+  <si>
+    <t>hillsdale</t>
+  </si>
+  <si>
+    <t>belmont</t>
+  </si>
+  <si>
+    <t>san_carlos</t>
+  </si>
+  <si>
+    <t>redwood_city</t>
+  </si>
+  <si>
+    <t>menlo_park</t>
+  </si>
+  <si>
+    <t>palo_alto</t>
+  </si>
+  <si>
+    <t>california_ave</t>
+  </si>
+  <si>
+    <t>san_antonio</t>
+  </si>
+  <si>
+    <t>mountain_view</t>
+  </si>
+  <si>
+    <t>sunnyvale</t>
+  </si>
+  <si>
+    <t>lawrence</t>
+  </si>
+  <si>
+    <t>santa_clara</t>
+  </si>
+  <si>
+    <t>sj_diridon</t>
+  </si>
+  <si>
+    <t>Stop Direction</t>
+  </si>
+  <si>
+    <t>Depart</t>
+  </si>
+  <si>
+    <t>Trip ID</t>
+  </si>
+  <si>
+    <t>Calendar service</t>
+  </si>
+  <si>
+    <t>Headsign</t>
+  </si>
+  <si>
+    <t>NYE-0100</t>
+  </si>
+  <si>
     <t>NYE</t>
-  </si>
-  <si>
-    <t>Direction</t>
-  </si>
-  <si>
-    <t>NYE-South</t>
-  </si>
-  <si>
-    <t>SF</t>
-  </si>
-  <si>
-    <t>22 St</t>
-  </si>
-  <si>
-    <t>Bayshore</t>
-  </si>
-  <si>
-    <t>S SF</t>
-  </si>
-  <si>
-    <t>San Bruno</t>
-  </si>
-  <si>
-    <t>Millbrae</t>
-  </si>
-  <si>
-    <t>Burlingame</t>
-  </si>
-  <si>
-    <t>San Mateo</t>
-  </si>
-  <si>
-    <t>Hayward Park</t>
-  </si>
-  <si>
-    <t>Hillsdale</t>
-  </si>
-  <si>
-    <t>Belmont</t>
-  </si>
-  <si>
-    <t>San Carlos</t>
-  </si>
-  <si>
-    <t>Redwood City</t>
-  </si>
-  <si>
-    <t>Menlo Park</t>
-  </si>
-  <si>
-    <t>Palo Alto</t>
-  </si>
-  <si>
-    <t>California Ave</t>
-  </si>
-  <si>
-    <t>San Antonio</t>
-  </si>
-  <si>
-    <t>Mountain View</t>
-  </si>
-  <si>
-    <t>Sunnyvale</t>
-  </si>
-  <si>
-    <t>Lawrence</t>
-  </si>
-  <si>
-    <t>Santa Clara</t>
-  </si>
-  <si>
-    <t>San Jose Diridon</t>
-  </si>
-  <si>
-    <t>Stop ID</t>
-  </si>
-  <si>
-    <t>Stop Direction</t>
-  </si>
-  <si>
-    <t>Depart</t>
-  </si>
-  <si>
-    <t>Trip ID</t>
-  </si>
-  <si>
-    <t>Calendar service</t>
-  </si>
-  <si>
-    <t>Headsign</t>
-  </si>
-  <si>
-    <t>NYE-0100</t>
   </si>
   <si>
     <t>NYE-0130</t>
@@ -410,243 +476,243 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
+      <c r="B2" s="1">
+        <v>1.0</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1">
-        <v>70012.0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>70022.0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>70032.0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>70042.0</v>
-      </c>
-      <c r="H3" s="1">
-        <v>70052.0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>70062.0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>70082.0</v>
-      </c>
-      <c r="K3" s="1">
-        <v>70092.0</v>
-      </c>
-      <c r="L3" s="2">
-        <v>70102.0</v>
-      </c>
-      <c r="M3" s="2">
-        <v>70112.0</v>
-      </c>
-      <c r="N3" s="2">
-        <v>70122.0</v>
-      </c>
-      <c r="O3" s="2">
-        <v>70132.0</v>
-      </c>
-      <c r="P3" s="2">
-        <v>70142.0</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>70162.0</v>
-      </c>
-      <c r="R3" s="2">
-        <v>70172.0</v>
-      </c>
-      <c r="S3" s="2">
-        <v>70192.0</v>
-      </c>
-      <c r="T3" s="2">
-        <v>70202.0</v>
-      </c>
-      <c r="U3" s="2">
-        <v>70212.0</v>
-      </c>
-      <c r="V3" s="2">
-        <v>70222.0</v>
-      </c>
-      <c r="W3" s="2">
-        <v>70232.0</v>
-      </c>
-      <c r="X3" s="2">
-        <v>70242.0</v>
-      </c>
-      <c r="Y3" s="2">
-        <v>70262.0</v>
+      <c r="E3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="4">
         <v>0.041666666666666664</v>
@@ -717,13 +783,13 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="5">
         <f t="shared" ref="D7:Y7" si="1">D6+TIME(0,30,0)</f>
@@ -816,13 +882,13 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" ref="D8:Y8" si="2">D6+TIME(1,0,0)</f>

</xml_diff>

<commit_message>
Switch to platform IDs for stop IDs
</commit_message>
<xml_diff>
--- a/input-data/NYE timetables.xlsx
+++ b/input-data/NYE timetables.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
   <si>
     <t>Route</t>
   </si>
@@ -89,72 +89,6 @@
   </si>
   <si>
     <t>Stop ID</t>
-  </si>
-  <si>
-    <t>san_francisco</t>
-  </si>
-  <si>
-    <t>22nd_street</t>
-  </si>
-  <si>
-    <t>bayshore</t>
-  </si>
-  <si>
-    <t>south_sf</t>
-  </si>
-  <si>
-    <t>san_bruno</t>
-  </si>
-  <si>
-    <t>millbrae</t>
-  </si>
-  <si>
-    <t>burlingame</t>
-  </si>
-  <si>
-    <t>san_mateo</t>
-  </si>
-  <si>
-    <t>hayward_park</t>
-  </si>
-  <si>
-    <t>hillsdale</t>
-  </si>
-  <si>
-    <t>belmont</t>
-  </si>
-  <si>
-    <t>san_carlos</t>
-  </si>
-  <si>
-    <t>redwood_city</t>
-  </si>
-  <si>
-    <t>menlo_park</t>
-  </si>
-  <si>
-    <t>palo_alto</t>
-  </si>
-  <si>
-    <t>california_ave</t>
-  </si>
-  <si>
-    <t>san_antonio</t>
-  </si>
-  <si>
-    <t>mountain_view</t>
-  </si>
-  <si>
-    <t>sunnyvale</t>
-  </si>
-  <si>
-    <t>lawrence</t>
-  </si>
-  <si>
-    <t>santa_clara</t>
-  </si>
-  <si>
-    <t>sj_diridon</t>
   </si>
   <si>
     <t>Stop Direction</t>
@@ -553,163 +487,163 @@
         <v>25</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>47</v>
+      <c r="D3" s="1">
+        <v>70012.0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>70022.0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>70032.0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>70042.0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>70052.0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>70062.0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>70082.0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>70092.0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>70102.0</v>
+      </c>
+      <c r="M3" s="2">
+        <v>70112.0</v>
+      </c>
+      <c r="N3" s="2">
+        <v>70122.0</v>
+      </c>
+      <c r="O3" s="2">
+        <v>70132.0</v>
+      </c>
+      <c r="P3" s="2">
+        <v>70142.0</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>70162.0</v>
+      </c>
+      <c r="R3" s="2">
+        <v>70172.0</v>
+      </c>
+      <c r="S3" s="2">
+        <v>70192.0</v>
+      </c>
+      <c r="T3" s="2">
+        <v>70202.0</v>
+      </c>
+      <c r="U3" s="2">
+        <v>70212.0</v>
+      </c>
+      <c r="V3" s="2">
+        <v>70222.0</v>
+      </c>
+      <c r="W3" s="2">
+        <v>70232.0</v>
+      </c>
+      <c r="X3" s="2">
+        <v>70242.0</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>70262.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>24</v>
@@ -783,10 +717,10 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>24</v>
@@ -882,10 +816,10 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>24</v>

</xml_diff>